<commit_message>
added axioms to allow for matching b/w bfo & ies.
</commit_message>
<xml_diff>
--- a/projects/project-3/assignment/src/data/bfo-axioms.xlsx
+++ b/projects/project-3/assignment/src/data/bfo-axioms.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b1</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b17</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -479,7 +479,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b20</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -492,7 +492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b23</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -505,7 +505,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b26</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb26</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -518,7 +518,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b29</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -531,7 +531,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b33</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb33</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -544,7 +544,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b37</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb37</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -557,7 +557,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b41</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb41</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -570,7 +570,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b45</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb45</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -583,7 +583,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b49</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb49</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -596,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b53</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb53</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -609,7 +609,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b56</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb56</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -622,7 +622,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b59</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -635,7 +635,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b66</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb66</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -648,7 +648,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b73</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb73</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -661,7 +661,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b77</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb77</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -674,7 +674,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b81</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb81</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -687,7 +687,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b84</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb84</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -700,7 +700,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b87</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb87</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -713,7 +713,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>na040bad41d1b44d5b512af38ea3674f3b9</t>
+          <t>n2e7a724ca8dc4fedaeaeed2f6551c45bb9</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>

</xml_diff>

<commit_message>
fixed errors in ccom & qudt definitions output
</commit_message>
<xml_diff>
--- a/projects/project-3/assignment/src/data/bfo-axioms.xlsx
+++ b/projects/project-3/assignment/src/data/bfo-axioms.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b1</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b17</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -479,7 +479,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b20</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -492,7 +492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b23</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -505,7 +505,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b26</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b26</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -518,7 +518,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b29</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -531,7 +531,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b33</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b33</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -544,7 +544,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b37</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b37</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -557,7 +557,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b41</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b41</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -570,7 +570,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b45</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b45</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -583,7 +583,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b49</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b49</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -596,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b53</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b53</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -609,7 +609,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b56</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b56</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -622,7 +622,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b59</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -635,7 +635,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b66</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b66</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -648,7 +648,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b73</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b73</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -661,7 +661,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b77</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b77</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -674,7 +674,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b81</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b81</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -687,7 +687,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b84</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b84</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -700,7 +700,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b87</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b87</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -713,7 +713,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>n425ac992496e4f4c872a808ed79f4ef9b9</t>
+          <t>n1e446dc28bab431fa3520a0ab74536d6b9</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>

</xml_diff>